<commit_message>
actualiza diccionarios de variables
</commit_message>
<xml_diff>
--- a/DataSets/ENGIH/ENGIH 2016 Codificador CCIF.xlsx
+++ b/DataSets/ENGIH/ENGIH 2016 Codificador CCIF.xlsx
@@ -8843,7 +8843,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="48.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19643,7 +19643,7 @@
         <v>2358</v>
       </c>
       <c r="G415" s="15">
-        <f>1/3</f>
+        <f t="shared" ref="G415:G446" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="H415" s="9" t="s">
@@ -19670,7 +19670,7 @@
         <v>2358</v>
       </c>
       <c r="G416" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H416" s="9" t="s">
@@ -19697,7 +19697,7 @@
         <v>2358</v>
       </c>
       <c r="G417" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H417" s="9" t="s">
@@ -19724,7 +19724,7 @@
         <v>2358</v>
       </c>
       <c r="G418" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H418" s="9" t="s">
@@ -19751,7 +19751,7 @@
         <v>2358</v>
       </c>
       <c r="G419" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H419" s="9" t="s">
@@ -19778,7 +19778,7 @@
         <v>2358</v>
       </c>
       <c r="G420" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H420" s="9" t="s">
@@ -19805,7 +19805,7 @@
         <v>2358</v>
       </c>
       <c r="G421" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H421" s="9" t="s">
@@ -19832,7 +19832,7 @@
         <v>2358</v>
       </c>
       <c r="G422" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H422" s="9" t="s">
@@ -19859,7 +19859,7 @@
         <v>2358</v>
       </c>
       <c r="G423" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H423" s="9" t="s">
@@ -19886,7 +19886,7 @@
         <v>2358</v>
       </c>
       <c r="G424" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H424" s="9" t="s">
@@ -19913,7 +19913,7 @@
         <v>2358</v>
       </c>
       <c r="G425" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H425" s="9" t="s">
@@ -19940,7 +19940,7 @@
         <v>2358</v>
       </c>
       <c r="G426" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H426" s="9" t="s">
@@ -19967,7 +19967,7 @@
         <v>2358</v>
       </c>
       <c r="G427" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H427" s="9" t="s">
@@ -19994,7 +19994,7 @@
         <v>2358</v>
       </c>
       <c r="G428" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H428" s="9" t="s">
@@ -20021,7 +20021,7 @@
         <v>2358</v>
       </c>
       <c r="G429" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H429" s="9" t="s">
@@ -20048,7 +20048,7 @@
         <v>2358</v>
       </c>
       <c r="G430" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H430" s="9" t="s">
@@ -20075,7 +20075,7 @@
         <v>2358</v>
       </c>
       <c r="G431" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H431" s="9" t="s">
@@ -20102,7 +20102,7 @@
         <v>2358</v>
       </c>
       <c r="G432" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H432" s="9" t="s">
@@ -20129,7 +20129,7 @@
         <v>2358</v>
       </c>
       <c r="G433" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H433" s="9" t="s">
@@ -20156,7 +20156,7 @@
         <v>2358</v>
       </c>
       <c r="G434" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H434" s="9" t="s">
@@ -20183,7 +20183,7 @@
         <v>2358</v>
       </c>
       <c r="G435" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H435" s="9" t="s">
@@ -20210,7 +20210,7 @@
         <v>2358</v>
       </c>
       <c r="G436" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H436" s="9" t="s">
@@ -20237,7 +20237,7 @@
         <v>2358</v>
       </c>
       <c r="G437" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H437" s="9" t="s">
@@ -20264,7 +20264,7 @@
         <v>2358</v>
       </c>
       <c r="G438" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H438" s="9" t="s">
@@ -20291,7 +20291,7 @@
         <v>2358</v>
       </c>
       <c r="G439" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H439" s="9" t="s">
@@ -20318,7 +20318,7 @@
         <v>2358</v>
       </c>
       <c r="G440" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H440" s="9" t="s">
@@ -20345,7 +20345,7 @@
         <v>2358</v>
       </c>
       <c r="G441" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H441" s="9" t="s">
@@ -20372,7 +20372,7 @@
         <v>2358</v>
       </c>
       <c r="G442" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H442" s="9" t="s">
@@ -20399,7 +20399,7 @@
         <v>2358</v>
       </c>
       <c r="G443" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H443" s="9" t="s">
@@ -20426,7 +20426,7 @@
         <v>2358</v>
       </c>
       <c r="G444" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H444" s="9" t="s">
@@ -20453,7 +20453,7 @@
         <v>2358</v>
       </c>
       <c r="G445" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H445" s="9" t="s">
@@ -20480,7 +20480,7 @@
         <v>2358</v>
       </c>
       <c r="G446" s="15">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H446" s="9" t="s">
@@ -20507,7 +20507,7 @@
         <v>2358</v>
       </c>
       <c r="G447" s="15">
-        <f>1/3</f>
+        <f t="shared" ref="G447:G467" si="1">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="H447" s="9" t="s">
@@ -20534,7 +20534,7 @@
         <v>2358</v>
       </c>
       <c r="G448" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H448" s="9" t="s">
@@ -20561,7 +20561,7 @@
         <v>2358</v>
       </c>
       <c r="G449" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H449" s="9" t="s">
@@ -20588,7 +20588,7 @@
         <v>2358</v>
       </c>
       <c r="G450" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H450" s="9" t="s">
@@ -20615,7 +20615,7 @@
         <v>2358</v>
       </c>
       <c r="G451" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H451" s="9" t="s">
@@ -20642,7 +20642,7 @@
         <v>2358</v>
       </c>
       <c r="G452" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H452" s="9" t="s">
@@ -20669,7 +20669,7 @@
         <v>2358</v>
       </c>
       <c r="G453" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H453" s="9" t="s">
@@ -20696,7 +20696,7 @@
         <v>2358</v>
       </c>
       <c r="G454" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H454" s="9" t="s">
@@ -20723,7 +20723,7 @@
         <v>2358</v>
       </c>
       <c r="G455" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H455" s="9" t="s">
@@ -20750,7 +20750,7 @@
         <v>2358</v>
       </c>
       <c r="G456" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H456" s="9" t="s">
@@ -20777,7 +20777,7 @@
         <v>2358</v>
       </c>
       <c r="G457" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H457" s="9" t="s">
@@ -20804,7 +20804,7 @@
         <v>2358</v>
       </c>
       <c r="G458" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H458" s="9" t="s">
@@ -20831,7 +20831,7 @@
         <v>2358</v>
       </c>
       <c r="G459" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H459" s="9" t="s">
@@ -20858,7 +20858,7 @@
         <v>2358</v>
       </c>
       <c r="G460" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H460" s="9" t="s">
@@ -20885,7 +20885,7 @@
         <v>2358</v>
       </c>
       <c r="G461" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H461" s="9" t="s">
@@ -20912,7 +20912,7 @@
         <v>2358</v>
       </c>
       <c r="G462" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H462" s="9" t="s">
@@ -20939,7 +20939,7 @@
         <v>2358</v>
       </c>
       <c r="G463" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H463" s="9" t="s">
@@ -20966,7 +20966,7 @@
         <v>2358</v>
       </c>
       <c r="G464" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H464" s="9" t="s">
@@ -20993,7 +20993,7 @@
         <v>2358</v>
       </c>
       <c r="G465" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H465" s="9" t="s">
@@ -21020,7 +21020,7 @@
         <v>2358</v>
       </c>
       <c r="G466" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H466" s="9" t="s">
@@ -21047,7 +21047,7 @@
         <v>2358</v>
       </c>
       <c r="G467" s="15">
-        <f>1/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H467" s="9" t="s">
@@ -21101,7 +21101,7 @@
         <v>2358</v>
       </c>
       <c r="G469" s="15">
-        <f>1/3</f>
+        <f t="shared" ref="G469:G487" si="2">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="H469" s="9" t="s">
@@ -21128,7 +21128,7 @@
         <v>2358</v>
       </c>
       <c r="G470" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H470" s="9" t="s">
@@ -21155,7 +21155,7 @@
         <v>2358</v>
       </c>
       <c r="G471" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H471" s="9" t="s">
@@ -21182,7 +21182,7 @@
         <v>2358</v>
       </c>
       <c r="G472" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H472" s="9" t="s">
@@ -21209,7 +21209,7 @@
         <v>2358</v>
       </c>
       <c r="G473" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H473" s="9" t="s">
@@ -21236,7 +21236,7 @@
         <v>2358</v>
       </c>
       <c r="G474" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H474" s="9" t="s">
@@ -21263,7 +21263,7 @@
         <v>2358</v>
       </c>
       <c r="G475" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H475" s="9" t="s">
@@ -21290,7 +21290,7 @@
         <v>2358</v>
       </c>
       <c r="G476" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H476" s="9" t="s">
@@ -21317,7 +21317,7 @@
         <v>2358</v>
       </c>
       <c r="G477" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H477" s="9" t="s">
@@ -21344,7 +21344,7 @@
         <v>2358</v>
       </c>
       <c r="G478" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H478" s="9" t="s">
@@ -21371,7 +21371,7 @@
         <v>2358</v>
       </c>
       <c r="G479" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H479" s="9" t="s">
@@ -21398,7 +21398,7 @@
         <v>2358</v>
       </c>
       <c r="G480" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H480" s="9" t="s">
@@ -21425,7 +21425,7 @@
         <v>2358</v>
       </c>
       <c r="G481" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H481" s="9" t="s">
@@ -21452,7 +21452,7 @@
         <v>2358</v>
       </c>
       <c r="G482" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H482" s="9" t="s">
@@ -21479,7 +21479,7 @@
         <v>2358</v>
       </c>
       <c r="G483" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H483" s="9" t="s">
@@ -21506,7 +21506,7 @@
         <v>2358</v>
       </c>
       <c r="G484" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H484" s="9" t="s">
@@ -21533,7 +21533,7 @@
         <v>2358</v>
       </c>
       <c r="G485" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H485" s="9" t="s">
@@ -21560,7 +21560,7 @@
         <v>2358</v>
       </c>
       <c r="G486" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H486" s="9" t="s">
@@ -21587,7 +21587,7 @@
         <v>2358</v>
       </c>
       <c r="G487" s="15">
-        <f>1/3</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H487" s="9" t="s">
@@ -21666,7 +21666,7 @@
         <v>2358</v>
       </c>
       <c r="G490" s="15">
-        <f>1/3</f>
+        <f t="shared" ref="G490:G517" si="3">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="H490" s="9" t="s">
@@ -21693,7 +21693,7 @@
         <v>2358</v>
       </c>
       <c r="G491" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H491" s="9" t="s">
@@ -21720,7 +21720,7 @@
         <v>2358</v>
       </c>
       <c r="G492" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H492" s="9" t="s">
@@ -21747,7 +21747,7 @@
         <v>2358</v>
       </c>
       <c r="G493" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H493" s="9" t="s">
@@ -21774,7 +21774,7 @@
         <v>2358</v>
       </c>
       <c r="G494" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H494" s="9" t="s">
@@ -21801,7 +21801,7 @@
         <v>2358</v>
       </c>
       <c r="G495" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H495" s="9" t="s">
@@ -21828,7 +21828,7 @@
         <v>2358</v>
       </c>
       <c r="G496" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H496" s="9" t="s">
@@ -21855,7 +21855,7 @@
         <v>2358</v>
       </c>
       <c r="G497" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H497" s="9" t="s">
@@ -21882,7 +21882,7 @@
         <v>2358</v>
       </c>
       <c r="G498" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H498" s="9" t="s">
@@ -21909,7 +21909,7 @@
         <v>2358</v>
       </c>
       <c r="G499" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H499" s="9" t="s">
@@ -21936,7 +21936,7 @@
         <v>2358</v>
       </c>
       <c r="G500" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H500" s="9" t="s">
@@ -21963,7 +21963,7 @@
         <v>2358</v>
       </c>
       <c r="G501" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H501" s="9" t="s">
@@ -21990,7 +21990,7 @@
         <v>2358</v>
       </c>
       <c r="G502" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H502" s="9" t="s">
@@ -22017,7 +22017,7 @@
         <v>2358</v>
       </c>
       <c r="G503" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H503" s="9" t="s">
@@ -22044,7 +22044,7 @@
         <v>2358</v>
       </c>
       <c r="G504" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H504" s="9" t="s">
@@ -22071,7 +22071,7 @@
         <v>2358</v>
       </c>
       <c r="G505" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H505" s="9" t="s">
@@ -22098,7 +22098,7 @@
         <v>2358</v>
       </c>
       <c r="G506" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H506" s="9" t="s">
@@ -22125,7 +22125,7 @@
         <v>2358</v>
       </c>
       <c r="G507" s="16">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H507" s="12" t="s">
@@ -22152,7 +22152,7 @@
         <v>2358</v>
       </c>
       <c r="G508" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H508" s="9" t="s">
@@ -22179,7 +22179,7 @@
         <v>2358</v>
       </c>
       <c r="G509" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H509" s="9" t="s">
@@ -22206,7 +22206,7 @@
         <v>2358</v>
       </c>
       <c r="G510" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H510" s="9" t="s">
@@ -22233,7 +22233,7 @@
         <v>2358</v>
       </c>
       <c r="G511" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H511" s="9" t="s">
@@ -22260,7 +22260,7 @@
         <v>2358</v>
       </c>
       <c r="G512" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H512" s="9" t="s">
@@ -22287,7 +22287,7 @@
         <v>2358</v>
       </c>
       <c r="G513" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H513" s="9" t="s">
@@ -22314,7 +22314,7 @@
         <v>2358</v>
       </c>
       <c r="G514" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H514" s="9" t="s">
@@ -22341,7 +22341,7 @@
         <v>2358</v>
       </c>
       <c r="G515" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H515" s="9" t="s">
@@ -22368,7 +22368,7 @@
         <v>2358</v>
       </c>
       <c r="G516" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H516" s="9" t="s">
@@ -22395,7 +22395,7 @@
         <v>2358</v>
       </c>
       <c r="G517" s="15">
-        <f>1/3</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H517" s="9" t="s">
@@ -22632,7 +22632,7 @@
         <v>2359</v>
       </c>
       <c r="G526" s="15">
-        <f>1/12</f>
+        <f t="shared" ref="G526:G544" si="4">1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H526" s="9" t="s">
@@ -22659,7 +22659,7 @@
         <v>2359</v>
       </c>
       <c r="G527" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H527" s="9" t="s">
@@ -22686,7 +22686,7 @@
         <v>2359</v>
       </c>
       <c r="G528" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H528" s="9" t="s">
@@ -22713,7 +22713,7 @@
         <v>2359</v>
       </c>
       <c r="G529" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H529" s="9" t="s">
@@ -22740,7 +22740,7 @@
         <v>2359</v>
       </c>
       <c r="G530" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H530" s="9" t="s">
@@ -22767,7 +22767,7 @@
         <v>2359</v>
       </c>
       <c r="G531" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H531" s="9" t="s">
@@ -22794,7 +22794,7 @@
         <v>2359</v>
       </c>
       <c r="G532" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H532" s="9" t="s">
@@ -22821,7 +22821,7 @@
         <v>2359</v>
       </c>
       <c r="G533" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H533" s="9" t="s">
@@ -22848,7 +22848,7 @@
         <v>2359</v>
       </c>
       <c r="G534" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H534" s="9" t="s">
@@ -22875,7 +22875,7 @@
         <v>2359</v>
       </c>
       <c r="G535" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H535" s="9" t="s">
@@ -22902,7 +22902,7 @@
         <v>2359</v>
       </c>
       <c r="G536" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H536" s="9" t="s">
@@ -22929,7 +22929,7 @@
         <v>2359</v>
       </c>
       <c r="G537" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H537" s="9" t="s">
@@ -22956,7 +22956,7 @@
         <v>2359</v>
       </c>
       <c r="G538" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H538" s="9" t="s">
@@ -22983,7 +22983,7 @@
         <v>2359</v>
       </c>
       <c r="G539" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H539" s="9" t="s">
@@ -23010,7 +23010,7 @@
         <v>2359</v>
       </c>
       <c r="G540" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H540" s="9" t="s">
@@ -23037,7 +23037,7 @@
         <v>2359</v>
       </c>
       <c r="G541" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H541" s="9" t="s">
@@ -23064,7 +23064,7 @@
         <v>2359</v>
       </c>
       <c r="G542" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H542" s="9" t="s">
@@ -23091,7 +23091,7 @@
         <v>2359</v>
       </c>
       <c r="G543" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H543" s="9" t="s">
@@ -23118,7 +23118,7 @@
         <v>2359</v>
       </c>
       <c r="G544" s="15">
-        <f>1/12</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H544" s="9" t="s">
@@ -23774,7 +23774,7 @@
         <v>2359</v>
       </c>
       <c r="G569" s="15">
-        <f>1/12</f>
+        <f t="shared" ref="G569:G588" si="5">1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H569" s="9" t="s">
@@ -23801,7 +23801,7 @@
         <v>2359</v>
       </c>
       <c r="G570" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H570" s="9" t="s">
@@ -23828,7 +23828,7 @@
         <v>2359</v>
       </c>
       <c r="G571" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H571" s="9" t="s">
@@ -23855,7 +23855,7 @@
         <v>2359</v>
       </c>
       <c r="G572" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H572" s="9" t="s">
@@ -23882,7 +23882,7 @@
         <v>2359</v>
       </c>
       <c r="G573" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H573" s="9" t="s">
@@ -23909,7 +23909,7 @@
         <v>2359</v>
       </c>
       <c r="G574" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H574" s="9" t="s">
@@ -23936,7 +23936,7 @@
         <v>2359</v>
       </c>
       <c r="G575" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H575" s="9" t="s">
@@ -23963,7 +23963,7 @@
         <v>2359</v>
       </c>
       <c r="G576" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H576" s="9" t="s">
@@ -23990,7 +23990,7 @@
         <v>2359</v>
       </c>
       <c r="G577" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H577" s="9" t="s">
@@ -24017,7 +24017,7 @@
         <v>2359</v>
       </c>
       <c r="G578" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H578" s="9" t="s">
@@ -24044,7 +24044,7 @@
         <v>2359</v>
       </c>
       <c r="G579" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H579" s="9" t="s">
@@ -24071,7 +24071,7 @@
         <v>2359</v>
       </c>
       <c r="G580" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H580" s="9" t="s">
@@ -24098,7 +24098,7 @@
         <v>2359</v>
       </c>
       <c r="G581" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H581" s="9" t="s">
@@ -24125,7 +24125,7 @@
         <v>2359</v>
       </c>
       <c r="G582" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H582" s="9" t="s">
@@ -24152,7 +24152,7 @@
         <v>2359</v>
       </c>
       <c r="G583" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H583" s="9" t="s">
@@ -24179,7 +24179,7 @@
         <v>2359</v>
       </c>
       <c r="G584" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H584" s="9" t="s">
@@ -24206,7 +24206,7 @@
         <v>2359</v>
       </c>
       <c r="G585" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H585" s="9" t="s">
@@ -24233,7 +24233,7 @@
         <v>2359</v>
       </c>
       <c r="G586" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H586" s="9" t="s">
@@ -24260,7 +24260,7 @@
         <v>2359</v>
       </c>
       <c r="G587" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H587" s="9" t="s">
@@ -24287,7 +24287,7 @@
         <v>2359</v>
       </c>
       <c r="G588" s="15">
-        <f>1/12</f>
+        <f t="shared" si="5"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H588" s="9" t="s">
@@ -24995,7 +24995,7 @@
         <v>2359</v>
       </c>
       <c r="G615" s="15">
-        <f>1/12</f>
+        <f t="shared" ref="G615:G647" si="6">1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H615" s="9" t="s">
@@ -25022,7 +25022,7 @@
         <v>2359</v>
       </c>
       <c r="G616" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H616" s="9" t="s">
@@ -25049,7 +25049,7 @@
         <v>2359</v>
       </c>
       <c r="G617" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H617" s="9" t="s">
@@ -25076,7 +25076,7 @@
         <v>2359</v>
       </c>
       <c r="G618" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H618" s="9" t="s">
@@ -25103,7 +25103,7 @@
         <v>2359</v>
       </c>
       <c r="G619" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H619" s="9" t="s">
@@ -25130,7 +25130,7 @@
         <v>2359</v>
       </c>
       <c r="G620" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H620" s="9" t="s">
@@ -25157,7 +25157,7 @@
         <v>2359</v>
       </c>
       <c r="G621" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H621" s="9" t="s">
@@ -25184,7 +25184,7 @@
         <v>2359</v>
       </c>
       <c r="G622" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H622" s="9" t="s">
@@ -25211,7 +25211,7 @@
         <v>2359</v>
       </c>
       <c r="G623" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H623" s="9" t="s">
@@ -25238,7 +25238,7 @@
         <v>2359</v>
       </c>
       <c r="G624" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H624" s="9" t="s">
@@ -25265,7 +25265,7 @@
         <v>2359</v>
       </c>
       <c r="G625" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H625" s="9" t="s">
@@ -25292,7 +25292,7 @@
         <v>2359</v>
       </c>
       <c r="G626" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H626" s="9" t="s">
@@ -25319,7 +25319,7 @@
         <v>2359</v>
       </c>
       <c r="G627" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H627" s="9" t="s">
@@ -25346,7 +25346,7 @@
         <v>2359</v>
       </c>
       <c r="G628" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H628" s="9" t="s">
@@ -25373,7 +25373,7 @@
         <v>2359</v>
       </c>
       <c r="G629" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H629" s="9" t="s">
@@ -25400,7 +25400,7 @@
         <v>2359</v>
       </c>
       <c r="G630" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H630" s="9" t="s">
@@ -25427,7 +25427,7 @@
         <v>2359</v>
       </c>
       <c r="G631" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H631" s="9" t="s">
@@ -25454,7 +25454,7 @@
         <v>2359</v>
       </c>
       <c r="G632" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H632" s="9" t="s">
@@ -25481,7 +25481,7 @@
         <v>2359</v>
       </c>
       <c r="G633" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H633" s="9" t="s">
@@ -25508,7 +25508,7 @@
         <v>2359</v>
       </c>
       <c r="G634" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H634" s="9" t="s">
@@ -25535,7 +25535,7 @@
         <v>2359</v>
       </c>
       <c r="G635" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H635" s="9" t="s">
@@ -25562,7 +25562,7 @@
         <v>2359</v>
       </c>
       <c r="G636" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H636" s="9" t="s">
@@ -25589,7 +25589,7 @@
         <v>2359</v>
       </c>
       <c r="G637" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H637" s="9" t="s">
@@ -25616,7 +25616,7 @@
         <v>2359</v>
       </c>
       <c r="G638" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H638" s="9" t="s">
@@ -25643,7 +25643,7 @@
         <v>2359</v>
       </c>
       <c r="G639" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H639" s="9" t="s">
@@ -25670,7 +25670,7 @@
         <v>2359</v>
       </c>
       <c r="G640" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H640" s="9" t="s">
@@ -25697,7 +25697,7 @@
         <v>2359</v>
       </c>
       <c r="G641" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H641" s="9" t="s">
@@ -25724,7 +25724,7 @@
         <v>2359</v>
       </c>
       <c r="G642" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H642" s="9" t="s">
@@ -25751,7 +25751,7 @@
         <v>2359</v>
       </c>
       <c r="G643" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H643" s="9" t="s">
@@ -25778,7 +25778,7 @@
         <v>2359</v>
       </c>
       <c r="G644" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H644" s="9" t="s">
@@ -25805,7 +25805,7 @@
         <v>2359</v>
       </c>
       <c r="G645" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H645" s="9" t="s">
@@ -25832,7 +25832,7 @@
         <v>2359</v>
       </c>
       <c r="G646" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H646" s="9" t="s">
@@ -25859,7 +25859,7 @@
         <v>2359</v>
       </c>
       <c r="G647" s="15">
-        <f>1/12</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H647" s="9" t="s">
@@ -25886,7 +25886,7 @@
         <v>2356</v>
       </c>
       <c r="G648" s="15">
-        <f>1/6</f>
+        <f t="shared" ref="G648:G676" si="7">1/6</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="H648" s="9" t="s">
@@ -25913,7 +25913,7 @@
         <v>2356</v>
       </c>
       <c r="G649" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H649" s="9" t="s">
@@ -25940,7 +25940,7 @@
         <v>2356</v>
       </c>
       <c r="G650" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H650" s="9" t="s">
@@ -25967,7 +25967,7 @@
         <v>2356</v>
       </c>
       <c r="G651" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H651" s="9" t="s">
@@ -25994,7 +25994,7 @@
         <v>2356</v>
       </c>
       <c r="G652" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H652" s="9" t="s">
@@ -26021,7 +26021,7 @@
         <v>2356</v>
       </c>
       <c r="G653" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H653" s="9" t="s">
@@ -26048,7 +26048,7 @@
         <v>2356</v>
       </c>
       <c r="G654" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H654" s="9" t="s">
@@ -26075,7 +26075,7 @@
         <v>2356</v>
       </c>
       <c r="G655" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H655" s="9" t="s">
@@ -26102,7 +26102,7 @@
         <v>2356</v>
       </c>
       <c r="G656" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H656" s="9" t="s">
@@ -26129,7 +26129,7 @@
         <v>2356</v>
       </c>
       <c r="G657" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H657" s="9" t="s">
@@ -26156,7 +26156,7 @@
         <v>2356</v>
       </c>
       <c r="G658" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H658" s="9" t="s">
@@ -26183,7 +26183,7 @@
         <v>2356</v>
       </c>
       <c r="G659" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H659" s="9" t="s">
@@ -26210,7 +26210,7 @@
         <v>2356</v>
       </c>
       <c r="G660" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H660" s="9" t="s">
@@ -26237,7 +26237,7 @@
         <v>2356</v>
       </c>
       <c r="G661" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H661" s="9" t="s">
@@ -26264,7 +26264,7 @@
         <v>2356</v>
       </c>
       <c r="G662" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H662" s="9" t="s">
@@ -26291,7 +26291,7 @@
         <v>2356</v>
       </c>
       <c r="G663" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H663" s="9" t="s">
@@ -26318,7 +26318,7 @@
         <v>2356</v>
       </c>
       <c r="G664" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H664" s="9" t="s">
@@ -26345,7 +26345,7 @@
         <v>2356</v>
       </c>
       <c r="G665" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H665" s="9" t="s">
@@ -26372,7 +26372,7 @@
         <v>2356</v>
       </c>
       <c r="G666" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H666" s="9" t="s">
@@ -26399,7 +26399,7 @@
         <v>2356</v>
       </c>
       <c r="G667" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H667" s="9" t="s">
@@ -26426,7 +26426,7 @@
         <v>2356</v>
       </c>
       <c r="G668" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H668" s="9" t="s">
@@ -26453,7 +26453,7 @@
         <v>2356</v>
       </c>
       <c r="G669" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H669" s="9" t="s">
@@ -26480,7 +26480,7 @@
         <v>2356</v>
       </c>
       <c r="G670" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H670" s="9" t="s">
@@ -26507,7 +26507,7 @@
         <v>2356</v>
       </c>
       <c r="G671" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H671" s="9" t="s">
@@ -26534,7 +26534,7 @@
         <v>2356</v>
       </c>
       <c r="G672" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H672" s="9" t="s">
@@ -26561,7 +26561,7 @@
         <v>2356</v>
       </c>
       <c r="G673" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H673" s="9" t="s">
@@ -26588,7 +26588,7 @@
         <v>2356</v>
       </c>
       <c r="G674" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H674" s="9" t="s">
@@ -26615,7 +26615,7 @@
         <v>2356</v>
       </c>
       <c r="G675" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H675" s="9" t="s">
@@ -26642,7 +26642,7 @@
         <v>2356</v>
       </c>
       <c r="G676" s="15">
-        <f>1/6</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H676" s="9" t="s">
@@ -28106,7 +28106,7 @@
         <v>2356</v>
       </c>
       <c r="G732" s="15">
-        <f>1/6</f>
+        <f t="shared" ref="G732:G741" si="8">1/6</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="H732" s="9" t="s">
@@ -28133,7 +28133,7 @@
         <v>2356</v>
       </c>
       <c r="G733" s="15">
-        <f>1/6</f>
+        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H733" s="9" t="s">
@@ -28160,7 +28160,7 @@
         <v>2356</v>
       </c>
       <c r="G734" s="15">
-        <f>1/6</f>
+        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H734" s="9" t="s">
@@ -28187,7 +28187,7 @@
         <v>2356</v>
       </c>
       <c r="G735" s="15">
-        <f>1/6</f>
+        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H735" s="9" t="s">
@@ -28214,7 +28214,7 @@
         <v>2356</v>
       </c>
       <c r="G736" s="15">
-        <f>1/6</f>
+        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H736" s="9" t="s">
@@ -28241,7 +28241,7 @@
         <v>2356</v>
       </c>
       <c r="G737" s="15">
-        <f>1/6</f>
+        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H737" s="9" t="s">
@@ -28268,7 +28268,7 @@
         <v>2356</v>
       </c>
       <c r="G738" s="15">
-        <f>1/6</f>
+        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H738" s="9" t="s">
@@ -28295,7 +28295,7 @@
         <v>2356</v>
       </c>
       <c r="G739" s="15">
-        <f>1/6</f>
+        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H739" s="9" t="s">
@@ -28322,7 +28322,7 @@
         <v>2356</v>
       </c>
       <c r="G740" s="15">
-        <f>1/6</f>
+        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H740" s="9" t="s">
@@ -28349,7 +28349,7 @@
         <v>2356</v>
       </c>
       <c r="G741" s="15">
-        <f>1/6</f>
+        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H741" s="9" t="s">
@@ -28428,7 +28428,7 @@
         <v>2358</v>
       </c>
       <c r="G744" s="15">
-        <f>1/3</f>
+        <f t="shared" ref="G744:G756" si="9">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="H744" s="9" t="s">
@@ -28455,7 +28455,7 @@
         <v>2358</v>
       </c>
       <c r="G745" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H745" s="9" t="s">
@@ -28482,7 +28482,7 @@
         <v>2358</v>
       </c>
       <c r="G746" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H746" s="9" t="s">
@@ -28509,7 +28509,7 @@
         <v>2358</v>
       </c>
       <c r="G747" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H747" s="9" t="s">
@@ -28536,7 +28536,7 @@
         <v>2358</v>
       </c>
       <c r="G748" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H748" s="9" t="s">
@@ -28563,7 +28563,7 @@
         <v>2358</v>
       </c>
       <c r="G749" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H749" s="9" t="s">
@@ -28590,7 +28590,7 @@
         <v>2358</v>
       </c>
       <c r="G750" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H750" s="9" t="s">
@@ -28617,7 +28617,7 @@
         <v>2358</v>
       </c>
       <c r="G751" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H751" s="9" t="s">
@@ -28644,7 +28644,7 @@
         <v>2358</v>
       </c>
       <c r="G752" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H752" s="9" t="s">
@@ -28671,7 +28671,7 @@
         <v>2358</v>
       </c>
       <c r="G753" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H753" s="9" t="s">
@@ -28698,7 +28698,7 @@
         <v>2358</v>
       </c>
       <c r="G754" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H754" s="9" t="s">
@@ -28725,7 +28725,7 @@
         <v>2358</v>
       </c>
       <c r="G755" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H755" s="9" t="s">
@@ -28752,7 +28752,7 @@
         <v>2358</v>
       </c>
       <c r="G756" s="15">
-        <f>1/3</f>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H756" s="9" t="s">
@@ -29169,7 +29169,7 @@
         <v>2359</v>
       </c>
       <c r="G772" s="15">
-        <f>1/12</f>
+        <f t="shared" ref="G772:G781" si="10">1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H772" s="9" t="s">
@@ -29196,7 +29196,7 @@
         <v>2359</v>
       </c>
       <c r="G773" s="15">
-        <f>1/12</f>
+        <f t="shared" si="10"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H773" s="9" t="s">
@@ -29223,7 +29223,7 @@
         <v>2359</v>
       </c>
       <c r="G774" s="15">
-        <f>1/12</f>
+        <f t="shared" si="10"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H774" s="9" t="s">
@@ -29250,7 +29250,7 @@
         <v>2359</v>
       </c>
       <c r="G775" s="15">
-        <f>1/12</f>
+        <f t="shared" si="10"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H775" s="9" t="s">
@@ -29277,7 +29277,7 @@
         <v>2359</v>
       </c>
       <c r="G776" s="15">
-        <f>1/12</f>
+        <f t="shared" si="10"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H776" s="9" t="s">
@@ -29304,7 +29304,7 @@
         <v>2359</v>
       </c>
       <c r="G777" s="15">
-        <f>1/12</f>
+        <f t="shared" si="10"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H777" s="9" t="s">
@@ -29331,7 +29331,7 @@
         <v>2359</v>
       </c>
       <c r="G778" s="15">
-        <f>1/12</f>
+        <f t="shared" si="10"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H778" s="9" t="s">
@@ -29358,7 +29358,7 @@
         <v>2359</v>
       </c>
       <c r="G779" s="15">
-        <f>1/12</f>
+        <f t="shared" si="10"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H779" s="9" t="s">
@@ -29385,7 +29385,7 @@
         <v>2359</v>
       </c>
       <c r="G780" s="15">
-        <f>1/12</f>
+        <f t="shared" si="10"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H780" s="9" t="s">
@@ -29412,7 +29412,7 @@
         <v>2359</v>
       </c>
       <c r="G781" s="15">
-        <f>1/12</f>
+        <f t="shared" si="10"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H781" s="9" t="s">
@@ -30212,7 +30212,7 @@
         <v>2356</v>
       </c>
       <c r="G811" s="15">
-        <f>1/6</f>
+        <f t="shared" ref="G811:G817" si="11">1/6</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="H811" s="9" t="s">
@@ -30239,7 +30239,7 @@
         <v>2356</v>
       </c>
       <c r="G812" s="15">
-        <f>1/6</f>
+        <f t="shared" si="11"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H812" s="9" t="s">
@@ -30266,7 +30266,7 @@
         <v>2356</v>
       </c>
       <c r="G813" s="15">
-        <f>1/6</f>
+        <f t="shared" si="11"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H813" s="9" t="s">
@@ -30293,7 +30293,7 @@
         <v>2356</v>
       </c>
       <c r="G814" s="15">
-        <f>1/6</f>
+        <f t="shared" si="11"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H814" s="9" t="s">
@@ -30320,7 +30320,7 @@
         <v>2356</v>
       </c>
       <c r="G815" s="15">
-        <f>1/6</f>
+        <f t="shared" si="11"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H815" s="9" t="s">
@@ -30347,7 +30347,7 @@
         <v>2356</v>
       </c>
       <c r="G816" s="15">
-        <f>1/6</f>
+        <f t="shared" si="11"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H816" s="9" t="s">
@@ -30374,7 +30374,7 @@
         <v>2356</v>
       </c>
       <c r="G817" s="15">
-        <f>1/6</f>
+        <f t="shared" si="11"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H817" s="9" t="s">
@@ -30982,7 +30982,7 @@
         <v>2359</v>
       </c>
       <c r="G840" s="15">
-        <f>1/12</f>
+        <f t="shared" ref="G840:G861" si="12">1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H840" s="9" t="s">
@@ -31009,7 +31009,7 @@
         <v>2359</v>
       </c>
       <c r="G841" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H841" s="9" t="s">
@@ -31036,7 +31036,7 @@
         <v>2359</v>
       </c>
       <c r="G842" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H842" s="9" t="s">
@@ -31063,7 +31063,7 @@
         <v>2359</v>
       </c>
       <c r="G843" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H843" s="9" t="s">
@@ -31090,7 +31090,7 @@
         <v>2359</v>
       </c>
       <c r="G844" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H844" s="9" t="s">
@@ -31117,7 +31117,7 @@
         <v>2359</v>
       </c>
       <c r="G845" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H845" s="9" t="s">
@@ -31144,7 +31144,7 @@
         <v>2359</v>
       </c>
       <c r="G846" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H846" s="9" t="s">
@@ -31171,7 +31171,7 @@
         <v>2359</v>
       </c>
       <c r="G847" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H847" s="9" t="s">
@@ -31198,7 +31198,7 @@
         <v>2359</v>
       </c>
       <c r="G848" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H848" s="9" t="s">
@@ -31225,7 +31225,7 @@
         <v>2359</v>
       </c>
       <c r="G849" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H849" s="9" t="s">
@@ -31252,7 +31252,7 @@
         <v>2359</v>
       </c>
       <c r="G850" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H850" s="9" t="s">
@@ -31279,7 +31279,7 @@
         <v>2359</v>
       </c>
       <c r="G851" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H851" s="9" t="s">
@@ -31306,7 +31306,7 @@
         <v>2359</v>
       </c>
       <c r="G852" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H852" s="9" t="s">
@@ -31333,7 +31333,7 @@
         <v>2359</v>
       </c>
       <c r="G853" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H853" s="9" t="s">
@@ -31360,7 +31360,7 @@
         <v>2359</v>
       </c>
       <c r="G854" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H854" s="9" t="s">
@@ -31387,7 +31387,7 @@
         <v>2359</v>
       </c>
       <c r="G855" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H855" s="9" t="s">
@@ -31414,7 +31414,7 @@
         <v>2359</v>
       </c>
       <c r="G856" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H856" s="9" t="s">
@@ -31441,7 +31441,7 @@
         <v>2359</v>
       </c>
       <c r="G857" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H857" s="9" t="s">
@@ -31468,7 +31468,7 @@
         <v>2359</v>
       </c>
       <c r="G858" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H858" s="9" t="s">
@@ -31495,7 +31495,7 @@
         <v>2359</v>
       </c>
       <c r="G859" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H859" s="9" t="s">
@@ -31522,7 +31522,7 @@
         <v>2359</v>
       </c>
       <c r="G860" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H860" s="9" t="s">
@@ -31549,7 +31549,7 @@
         <v>2359</v>
       </c>
       <c r="G861" s="15">
-        <f>1/12</f>
+        <f t="shared" si="12"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H861" s="9" t="s">
@@ -39068,7 +39068,7 @@
         <v>2356</v>
       </c>
       <c r="G1149" s="15">
-        <f>1/6</f>
+        <f t="shared" ref="G1149:G1154" si="13">1/6</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="H1149" s="9" t="s">
@@ -39095,7 +39095,7 @@
         <v>2356</v>
       </c>
       <c r="G1150" s="15">
-        <f>1/6</f>
+        <f t="shared" si="13"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H1150" s="9" t="s">
@@ -39122,7 +39122,7 @@
         <v>2356</v>
       </c>
       <c r="G1151" s="15">
-        <f>1/6</f>
+        <f t="shared" si="13"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H1151" s="9" t="s">
@@ -39149,7 +39149,7 @@
         <v>2356</v>
       </c>
       <c r="G1152" s="15">
-        <f>1/6</f>
+        <f t="shared" si="13"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H1152" s="9" t="s">
@@ -39176,7 +39176,7 @@
         <v>2356</v>
       </c>
       <c r="G1153" s="15">
-        <f>1/6</f>
+        <f t="shared" si="13"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H1153" s="9" t="s">
@@ -39203,7 +39203,7 @@
         <v>2356</v>
       </c>
       <c r="G1154" s="15">
-        <f>1/6</f>
+        <f t="shared" si="13"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H1154" s="9" t="s">
@@ -40782,7 +40782,7 @@
         <v>2359</v>
       </c>
       <c r="G1214" s="15">
-        <f>1/12</f>
+        <f t="shared" ref="G1214:G1220" si="14">1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1214" s="9" t="s">
@@ -40809,7 +40809,7 @@
         <v>2359</v>
       </c>
       <c r="G1215" s="15">
-        <f>1/12</f>
+        <f t="shared" si="14"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1215" s="9" t="s">
@@ -40836,7 +40836,7 @@
         <v>2359</v>
       </c>
       <c r="G1216" s="15">
-        <f>1/12</f>
+        <f t="shared" si="14"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1216" s="9" t="s">
@@ -40863,7 +40863,7 @@
         <v>2359</v>
       </c>
       <c r="G1217" s="15">
-        <f>1/12</f>
+        <f t="shared" si="14"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1217" s="9" t="s">
@@ -40890,7 +40890,7 @@
         <v>2359</v>
       </c>
       <c r="G1218" s="15">
-        <f>1/12</f>
+        <f t="shared" si="14"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1218" s="9" t="s">
@@ -40917,7 +40917,7 @@
         <v>2359</v>
       </c>
       <c r="G1219" s="15">
-        <f>1/12</f>
+        <f t="shared" si="14"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1219" s="9" t="s">
@@ -40944,7 +40944,7 @@
         <v>2359</v>
       </c>
       <c r="G1220" s="15">
-        <f>1/12</f>
+        <f t="shared" si="14"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1220" s="9" t="s">
@@ -41104,7 +41104,7 @@
         <v>2359</v>
       </c>
       <c r="G1226" s="15">
-        <f>1/12</f>
+        <f t="shared" ref="G1226:G1233" si="15">1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1226" s="9" t="s">
@@ -41131,7 +41131,7 @@
         <v>2359</v>
       </c>
       <c r="G1227" s="15">
-        <f>1/12</f>
+        <f t="shared" si="15"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1227" s="9" t="s">
@@ -41158,7 +41158,7 @@
         <v>2359</v>
       </c>
       <c r="G1228" s="15">
-        <f>1/12</f>
+        <f t="shared" si="15"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1228" s="9" t="s">
@@ -41185,7 +41185,7 @@
         <v>2359</v>
       </c>
       <c r="G1229" s="15">
-        <f>1/12</f>
+        <f t="shared" si="15"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1229" s="9" t="s">
@@ -41212,7 +41212,7 @@
         <v>2359</v>
       </c>
       <c r="G1230" s="15">
-        <f>1/12</f>
+        <f t="shared" si="15"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1230" s="9" t="s">
@@ -41239,7 +41239,7 @@
         <v>2359</v>
       </c>
       <c r="G1231" s="15">
-        <f>1/12</f>
+        <f t="shared" si="15"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1231" s="9" t="s">
@@ -41266,7 +41266,7 @@
         <v>2359</v>
       </c>
       <c r="G1232" s="15">
-        <f>1/12</f>
+        <f t="shared" si="15"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1232" s="9" t="s">
@@ -41293,7 +41293,7 @@
         <v>2359</v>
       </c>
       <c r="G1233" s="15">
-        <f>1/12</f>
+        <f t="shared" si="15"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1233" s="9" t="s">
@@ -41424,7 +41424,7 @@
         <v>2359</v>
       </c>
       <c r="G1238" s="16">
-        <f>1/12</f>
+        <f t="shared" ref="G1238:G1244" si="16">1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1238" s="12" t="s">
@@ -41451,7 +41451,7 @@
         <v>2359</v>
       </c>
       <c r="G1239" s="15">
-        <f>1/12</f>
+        <f t="shared" si="16"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1239" s="9" t="s">
@@ -41478,7 +41478,7 @@
         <v>2359</v>
       </c>
       <c r="G1240" s="15">
-        <f>1/12</f>
+        <f t="shared" si="16"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1240" s="9" t="s">
@@ -41505,7 +41505,7 @@
         <v>2359</v>
       </c>
       <c r="G1241" s="15">
-        <f>1/12</f>
+        <f t="shared" si="16"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1241" s="9" t="s">
@@ -41532,7 +41532,7 @@
         <v>2359</v>
       </c>
       <c r="G1242" s="15">
-        <f>1/12</f>
+        <f t="shared" si="16"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1242" s="9" t="s">
@@ -41559,7 +41559,7 @@
         <v>2359</v>
       </c>
       <c r="G1243" s="15">
-        <f>1/12</f>
+        <f t="shared" si="16"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1243" s="9" t="s">
@@ -41586,7 +41586,7 @@
         <v>2359</v>
       </c>
       <c r="G1244" s="15">
-        <f>1/12</f>
+        <f t="shared" si="16"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1244" s="9" t="s">
@@ -41665,7 +41665,7 @@
         <v>2359</v>
       </c>
       <c r="G1247" s="16">
-        <f>1/12</f>
+        <f t="shared" ref="G1247:G1259" si="17">1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1247" s="12" t="s">
@@ -41692,7 +41692,7 @@
         <v>2359</v>
       </c>
       <c r="G1248" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1248" s="9" t="s">
@@ -41719,7 +41719,7 @@
         <v>2359</v>
       </c>
       <c r="G1249" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1249" s="9" t="s">
@@ -41746,7 +41746,7 @@
         <v>2359</v>
       </c>
       <c r="G1250" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1250" s="9" t="s">
@@ -41773,7 +41773,7 @@
         <v>2359</v>
       </c>
       <c r="G1251" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1251" s="9" t="s">
@@ -41800,7 +41800,7 @@
         <v>2359</v>
       </c>
       <c r="G1252" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1252" s="9" t="s">
@@ -41827,7 +41827,7 @@
         <v>2359</v>
       </c>
       <c r="G1253" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1253" s="9" t="s">
@@ -41854,7 +41854,7 @@
         <v>2359</v>
       </c>
       <c r="G1254" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1254" s="9" t="s">
@@ -41881,7 +41881,7 @@
         <v>2359</v>
       </c>
       <c r="G1255" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1255" s="9" t="s">
@@ -41908,7 +41908,7 @@
         <v>2359</v>
       </c>
       <c r="G1256" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1256" s="9" t="s">
@@ -41935,7 +41935,7 @@
         <v>2359</v>
       </c>
       <c r="G1257" s="16">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1257" s="12" t="s">
@@ -41962,7 +41962,7 @@
         <v>2359</v>
       </c>
       <c r="G1258" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1258" s="9" t="s">
@@ -41989,7 +41989,7 @@
         <v>2359</v>
       </c>
       <c r="G1259" s="15">
-        <f>1/12</f>
+        <f t="shared" si="17"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H1259" s="9" t="s">

</xml_diff>